<commit_message>
T1: Refactored and added testCases for teachers
</commit_message>
<xml_diff>
--- a/PIO_DPU_Slownik_Scenariusz/Testy_Przypadki.xlsx
+++ b/PIO_DPU_Slownik_Scenariusz/Testy_Przypadki.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8205"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="student" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="172">
   <si>
     <t>lp</t>
   </si>
@@ -264,51 +264,15 @@
     <t>000000@student.pwr.wroc.3</t>
   </si>
   <si>
-    <t>wczesniejOk_adresSerwera4_znak</t>
-  </si>
-  <si>
     <t>wczesniejOk_adresSerwera4_cyfra</t>
   </si>
   <si>
-    <t>000000@student.pwr.wroc.a</t>
-  </si>
-  <si>
-    <t>wczesniejOk_adresSerwera4_2_znak</t>
-  </si>
-  <si>
-    <t>000000@student.pwr.wroc.ab</t>
-  </si>
-  <si>
-    <t>wczesniejOk_adresSerwera4_2_cyfra</t>
-  </si>
-  <si>
-    <t>000000@student.pwr.wroc.33</t>
-  </si>
-  <si>
     <t>wczesniejOk_adresSerwera4_com</t>
   </si>
   <si>
     <t>000000@student.pwr.wroc.com</t>
   </si>
   <si>
-    <t>syntaktyka</t>
-  </si>
-  <si>
-    <t>najpierw</t>
-  </si>
-  <si>
-    <t>semantyka</t>
-  </si>
-  <si>
-    <t>potem</t>
-  </si>
-  <si>
-    <t>nazwa_Konta_5_Cyfr_1_Spacja</t>
-  </si>
-  <si>
-    <t>asdzxc @student.pwr.edu.pl</t>
-  </si>
-  <si>
     <t>wczesniejOk_adresSerwera1_spacja</t>
   </si>
   <si>
@@ -330,9 +294,6 @@
     <t>wczesniejOk_adresSerwera4_spacja</t>
   </si>
   <si>
-    <t xml:space="preserve">000000@student.pwr.wroc. </t>
-  </si>
-  <si>
     <t>spacja</t>
   </si>
   <si>
@@ -340,6 +301,246 @@
   </si>
   <si>
     <t>Syntaktyka</t>
+  </si>
+  <si>
+    <t>nazwa_Konta_6_Cyfr_1_Spacja</t>
+  </si>
+  <si>
+    <t>000001 @student.pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>000000@student.pwr.wroc. pl</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera4_pd</t>
+  </si>
+  <si>
+    <t>000000@student.pwr.wroc.pd</t>
+  </si>
+  <si>
+    <t>"@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera1_brak</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera1_1_znak</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera1_1_cyfra</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera1_2_cyfra</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera2_2_znak</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera2_2_znak_1_cyfra</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera2_4_znak</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera2_dobry_aliasWroc</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera3_pd</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera3_cyfra</t>
+  </si>
+  <si>
+    <t>wczesniejOk_adresSerwera3_com</t>
+  </si>
+  <si>
+    <t>ala.nowak@@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak @pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowakpwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@..pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@ .edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@a.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@3.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@32.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr. .pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr..pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.a.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.3.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.aa.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.33.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.aa3.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.aaaa.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.wroc.pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.wroc. pl</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.wroc.pd</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.wroc.3</t>
+  </si>
+  <si>
+    <t>ala.nowak@pwr.wroc.com</t>
+  </si>
+  <si>
+    <t>nazwaKonta2</t>
+  </si>
+  <si>
+    <t>nazwaKonta1</t>
+  </si>
+  <si>
+    <t>ala</t>
+  </si>
+  <si>
+    <t>nowak</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1y2_0_Znakow</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1_1_Znak</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1_1_Cyfra</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1_2_Cyfry</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1_6_Cyfry</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1_7_Cyfry</t>
+  </si>
+  <si>
+    <t>nazwa_Konta2_1_Znak</t>
+  </si>
+  <si>
+    <t>nazwa_Konta2_1_Cyfra</t>
+  </si>
+  <si>
+    <t>nazwa_Konta2_2_Cyfry</t>
+  </si>
+  <si>
+    <t>nazwa_Konta2_6_Cyfry</t>
+  </si>
+  <si>
+    <t>nazwa_Konta2_7_Cyfry</t>
+  </si>
+  <si>
+    <t>nazwa_Konta2_5_Cyfry_1_Znak</t>
+  </si>
+  <si>
+    <t>nazwa_Konta2_6_Znakow</t>
+  </si>
+  <si>
+    <t>wczesniejOk_6_Cyfr_2xMalpa</t>
+  </si>
+  <si>
+    <t>wczesniejOk_Cyfr_1_Spacja</t>
+  </si>
+  <si>
+    <t>wczesniejOk_Cyfr_BrakMalpy</t>
+  </si>
+  <si>
+    <t>ala.a@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.2@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.23@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.000000@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.0000000@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.000001@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.00000a@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>ala.asdzxc@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>a.ala@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>2.ala@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>23.ala@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>000000.ala@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>0000000.ala@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>00000a.ala@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>asdzxc.ala@pwr.edu.pl</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1y2_6_Cyfry</t>
+  </si>
+  <si>
+    <t>ponad64_nazwaUzytkownika</t>
+  </si>
+  <si>
+    <t>alaasdasdasdasdasdasdsdfasdfasdf.nowakasdfasdfasdfasdfasdfasdfasdfasdfasdfasdfasdfasdfasdf@pwr.wroc.com</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1_5_Cyfry_1_Znak</t>
+  </si>
+  <si>
+    <t>nazwa_Konta1_6_Znakow</t>
   </si>
 </sst>
 </file>
@@ -395,7 +596,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -486,21 +687,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -553,6 +739,75 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -564,7 +819,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -577,17 +832,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -871,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D48" sqref="A1:D48"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,17 +1148,17 @@
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="A1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15"/>
       <c r="G1" t="s">
         <v>5</v>
       </c>
@@ -928,7 +1191,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>21</v>
@@ -946,7 +1209,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>22</v>
@@ -962,9 +1225,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>3</v>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>23</v>
@@ -980,17 +1243,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>3</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="21"/>
       <c r="G6" t="s">
         <v>14</v>
       </c>
@@ -999,8 +1262,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>5</v>
+      <c r="A7" s="17">
+        <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>27</v>
@@ -1018,7 +1281,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>47</v>
@@ -1030,7 +1293,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>27</v>
@@ -1042,7 +1305,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>36</v>
@@ -1051,16 +1314,10 @@
         <v>37</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="F10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>30</v>
@@ -1069,18 +1326,12 @@
         <v>31</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="F11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22">
+        <v>9</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1088,11 +1339,11 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22">
+        <v>10</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>92</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1100,11 +1351,11 @@
       </c>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22">
+        <v>11</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1112,11 +1363,11 @@
       </c>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7" t="s">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
+        <v>12</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1124,9 +1375,9 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>40</v>
@@ -1134,23 +1385,23 @@
       <c r="C16" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22">
+        <v>14</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <v>15</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>43</v>
@@ -1160,11 +1411,11 @@
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>17</v>
-      </c>
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22">
+        <v>16</v>
+      </c>
+      <c r="B19" s="23" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -1174,7 +1425,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>50</v>
@@ -1184,9 +1435,9 @@
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>19</v>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22">
+        <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>51</v>
@@ -1196,327 +1447,288 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
         <v>20</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="B23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22">
+        <v>22</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22">
+        <v>23</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="22">
+        <v>24</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22">
+        <v>25</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22">
+        <v>26</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22">
+        <v>27</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22">
+        <v>28</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22">
+        <v>29</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="22">
+        <v>30</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22">
+        <v>31</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="22">
+        <v>32</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22">
+        <v>33</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="22">
+        <v>34</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="22">
+        <v>35</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22">
+        <v>36</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="22">
+        <v>37</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>96</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>22</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>23</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>24</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>25</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>26</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>27</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <v>28</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>29</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <v>30</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <v>31</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
-        <v>32</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
-        <v>33</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>34</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
-        <v>35</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
-        <v>36</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="10"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
-        <v>37</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
-        <v>38</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
+        <v>38</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="22">
         <v>39</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" s="10"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
-        <v>40</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>80</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D42" s="8"/>
+        <v>81</v>
+      </c>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
+        <v>40</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
         <v>41</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
-        <v>42</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D44" s="10"/>
+      <c r="B44" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
-        <v>43</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
-        <v>44</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" s="8"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
-        <v>45</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="8"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="11">
-        <v>46</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D48" s="13"/>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1538,14 +1750,14 @@
     <hyperlink ref="C18" r:id="rId13"/>
     <hyperlink ref="C19" r:id="rId14"/>
     <hyperlink ref="C20" r:id="rId15"/>
-    <hyperlink ref="C21" r:id="rId16"/>
-    <hyperlink ref="C8" r:id="rId17"/>
-    <hyperlink ref="C22" r:id="rId18"/>
+    <hyperlink ref="C8" r:id="rId16"/>
+    <hyperlink ref="C21" r:id="rId17"/>
+    <hyperlink ref="C23" r:id="rId18"/>
     <hyperlink ref="C24" r:id="rId19"/>
     <hyperlink ref="C25" r:id="rId20"/>
     <hyperlink ref="C26" r:id="rId21"/>
     <hyperlink ref="C27" r:id="rId22"/>
-    <hyperlink ref="C28" r:id="rId23"/>
+    <hyperlink ref="C29" r:id="rId23"/>
     <hyperlink ref="C30" r:id="rId24"/>
     <hyperlink ref="C31" r:id="rId25"/>
     <hyperlink ref="C32" r:id="rId26"/>
@@ -1554,19 +1766,15 @@
     <hyperlink ref="C35" r:id="rId29"/>
     <hyperlink ref="C36" r:id="rId30"/>
     <hyperlink ref="C37" r:id="rId31"/>
-    <hyperlink ref="C38" r:id="rId32"/>
-    <hyperlink ref="C39" r:id="rId33"/>
-    <hyperlink ref="C41" r:id="rId34"/>
-    <hyperlink ref="C42" r:id="rId35"/>
-    <hyperlink ref="C43" r:id="rId36"/>
-    <hyperlink ref="C44" r:id="rId37"/>
-    <hyperlink ref="C45" r:id="rId38"/>
-    <hyperlink ref="C46" r:id="rId39"/>
-    <hyperlink ref="C13" r:id="rId40" display="asdzxc@student.pwr.edu.pl"/>
-    <hyperlink ref="C17" r:id="rId41"/>
-    <hyperlink ref="C23" r:id="rId42"/>
-    <hyperlink ref="C29" r:id="rId43"/>
-    <hyperlink ref="C40" r:id="rId44"/>
+    <hyperlink ref="C40" r:id="rId32"/>
+    <hyperlink ref="C41" r:id="rId33"/>
+    <hyperlink ref="C42" r:id="rId34"/>
+    <hyperlink ref="C13" r:id="rId35" display="asdzxc@student.pwr.edu.pl"/>
+    <hyperlink ref="C17" r:id="rId36"/>
+    <hyperlink ref="C22" r:id="rId37"/>
+    <hyperlink ref="C28" r:id="rId38"/>
+    <hyperlink ref="C38" r:id="rId39"/>
+    <hyperlink ref="C39" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1574,12 +1782,684 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15"/>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="G3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>3</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22">
+        <v>10</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22">
+        <v>14</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>15</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>17</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22">
+        <v>18</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>20</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22">
+        <v>21</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22">
+        <v>22</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="22">
+        <v>23</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="22">
+        <v>24</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22">
+        <v>25</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22">
+        <v>26</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22">
+        <v>27</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22">
+        <v>28</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22">
+        <v>29</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="22">
+        <v>30</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22">
+        <v>31</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="22">
+        <v>32</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="22">
+        <v>33</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="22">
+        <v>34</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="22">
+        <v>35</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22">
+        <v>36</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="22">
+        <v>37</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
+        <v>38</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" s="10"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="22">
+        <v>39</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>40</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>41</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="22">
+        <v>42</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>43</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
+        <v>44</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="22">
+        <v>45</v>
+      </c>
+      <c r="D48" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId2"/>
+    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="C15" r:id="rId4"/>
+    <hyperlink ref="C13" r:id="rId5"/>
+    <hyperlink ref="C19" r:id="rId6"/>
+    <hyperlink ref="C18" r:id="rId7"/>
+    <hyperlink ref="C20" r:id="rId8" display="000001@student.pwr.edu.pl"/>
+    <hyperlink ref="C22" r:id="rId9" display="000001@student.pwr.edu.pl"/>
+    <hyperlink ref="C17" r:id="rId10"/>
+    <hyperlink ref="C16" r:id="rId11"/>
+    <hyperlink ref="C23" r:id="rId12"/>
+    <hyperlink ref="C25" r:id="rId13"/>
+    <hyperlink ref="C26" r:id="rId14"/>
+    <hyperlink ref="C27" r:id="rId15"/>
+    <hyperlink ref="C28" r:id="rId16"/>
+    <hyperlink ref="C29" r:id="rId17"/>
+    <hyperlink ref="C31" r:id="rId18"/>
+    <hyperlink ref="C32" r:id="rId19"/>
+    <hyperlink ref="C33" r:id="rId20"/>
+    <hyperlink ref="C34" r:id="rId21"/>
+    <hyperlink ref="C35" r:id="rId22"/>
+    <hyperlink ref="C36" r:id="rId23"/>
+    <hyperlink ref="C37" r:id="rId24"/>
+    <hyperlink ref="C38" r:id="rId25"/>
+    <hyperlink ref="C39" r:id="rId26"/>
+    <hyperlink ref="C42" r:id="rId27"/>
+    <hyperlink ref="C43" r:id="rId28"/>
+    <hyperlink ref="C44" r:id="rId29"/>
+    <hyperlink ref="C21" r:id="rId30" display="asdzxc@student.pwr.edu.pl"/>
+    <hyperlink ref="C24" r:id="rId31"/>
+    <hyperlink ref="C30" r:id="rId32"/>
+    <hyperlink ref="C40" r:id="rId33"/>
+    <hyperlink ref="C41" r:id="rId34"/>
+    <hyperlink ref="C4" r:id="rId35"/>
+    <hyperlink ref="C5" r:id="rId36"/>
+    <hyperlink ref="C7" r:id="rId37"/>
+    <hyperlink ref="C6" r:id="rId38"/>
+    <hyperlink ref="C10" r:id="rId39"/>
+    <hyperlink ref="C9" r:id="rId40"/>
+    <hyperlink ref="C8" r:id="rId41"/>
+    <hyperlink ref="C14" r:id="rId42"/>
+    <hyperlink ref="C45" r:id="rId43"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>